<commit_message>
Added note on the bubble charts
</commit_message>
<xml_diff>
--- a/ProcessedData/Coaches_Summary/nfl coach summary.xlsx
+++ b/ProcessedData/Coaches_Summary/nfl coach summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23070" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="23070" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -1525,9 +1525,6 @@
     <t>See the "Yearly Heatmap" sheet for a visual aid explaining how NFL stats have evolved by year. Note that it only includes 16 game seasons.</t>
   </si>
   <si>
-    <t>I plotted Oscore_Rank, Dscore_Rank, Stscore_Rank, and GampeControlPlusBalance_Rank in RankCharts. Check them out.</t>
-  </si>
-  <si>
     <t>Cross-referencing each coach's history (as head coach or coordinator), I compiled their seasonal averages, including their coached team's average rank in many different categories, sortable.</t>
   </si>
   <si>
@@ -1594,6 +1591,9 @@
   </si>
   <si>
     <t>Ever wonder how good your favorite NFL team's head coach and coordinators are, and wish you had some data to form an opinion?</t>
+  </si>
+  <si>
+    <t>I plotted Oscore_Rank, Dscore_Rank, Stscore_Rank, and GampeControlPlusBalance_Rank in RankCharts. Check them out. For best viewing results, sort the coaches alphabetically in their respective tables.</t>
   </si>
 </sst>
 </file>
@@ -2573,11 +2573,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="386842048"/>
-        <c:axId val="386836952"/>
+        <c:axId val="397344784"/>
+        <c:axId val="397337728"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="386842048"/>
+        <c:axId val="397344784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="58"/>
@@ -2671,12 +2671,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="386836952"/>
+        <c:crossAx val="397337728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="386836952"/>
+        <c:axId val="397337728"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="28"/>
@@ -2796,7 +2796,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386842048"/>
+        <c:crossAx val="397344784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3670,11 +3670,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="477249544"/>
-        <c:axId val="477252680"/>
+        <c:axId val="397339296"/>
+        <c:axId val="397339688"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="477249544"/>
+        <c:axId val="397339296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="63"/>
@@ -3767,12 +3767,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="477252680"/>
+        <c:crossAx val="397339688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="477252680"/>
+        <c:axId val="397339688"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="32"/>
@@ -3891,7 +3891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477249544"/>
+        <c:crossAx val="397339296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4439,11 +4439,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="477251896"/>
-        <c:axId val="477249936"/>
+        <c:axId val="397340080"/>
+        <c:axId val="397341256"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="477251896"/>
+        <c:axId val="397340080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4530,12 +4530,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="477249936"/>
+        <c:crossAx val="397341256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="477249936"/>
+        <c:axId val="397341256"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="32"/>
@@ -4650,7 +4650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477251896"/>
+        <c:crossAx val="397340080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5146,11 +5146,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="477248760"/>
-        <c:axId val="477246800"/>
+        <c:axId val="502715864"/>
+        <c:axId val="502714296"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="477248760"/>
+        <c:axId val="502715864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -5243,12 +5243,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="477246800"/>
+        <c:crossAx val="502714296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="477246800"/>
+        <c:axId val="502714296"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="30"/>
@@ -5368,7 +5368,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477248760"/>
+        <c:crossAx val="502715864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9031,8 +9031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9061,7 +9061,7 @@
     <row r="3" spans="1:21" ht="336.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -9083,7 +9083,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -9103,12 +9103,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -9133,22 +9133,22 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -9213,12 +9213,12 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -9253,7 +9253,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -9271,7 +9271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -85276,7 +85276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -85456,10 +85456,10 @@
         <v>158</v>
       </c>
       <c r="AX1" t="s">
+        <v>509</v>
+      </c>
+      <c r="AY1" t="s">
         <v>510</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>511</v>
       </c>
       <c r="AZ1" t="s">
         <v>151</v>
@@ -85564,7 +85564,7 @@
         <v>110</v>
       </c>
       <c r="CH1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="CI1" t="s">
         <v>405</v>
@@ -94364,7 +94364,7 @@
     </row>
     <row r="36" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>